<commit_message>
update prep_palm_input_update & outputs
</commit_message>
<xml_diff>
--- a/code/h1_data_left.xlsx
+++ b/code/h1_data_left.xlsx
@@ -13,7 +13,1393 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="686">
+  <si>
+    <t>IV_avg</t>
+  </si>
+  <si>
+    <t>V_avg</t>
+  </si>
+  <si>
+    <t>VI_avg</t>
+  </si>
+  <si>
+    <t>Crus_I_avg</t>
+  </si>
+  <si>
+    <t>Crus_II_avg</t>
+  </si>
+  <si>
+    <t>VIIb_avg</t>
+  </si>
+  <si>
+    <t>VIIIa_avg</t>
+  </si>
+  <si>
+    <t>VIIIb_avg</t>
+  </si>
+  <si>
+    <t>IX_avg</t>
+  </si>
+  <si>
+    <t>X_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VI_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIa_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIb_avg</t>
+  </si>
+  <si>
+    <t>Vermis_IX_avg</t>
+  </si>
+  <si>
+    <t>IV_avg</t>
+  </si>
+  <si>
+    <t>V_avg</t>
+  </si>
+  <si>
+    <t>VI_avg</t>
+  </si>
+  <si>
+    <t>Crus_I_avg</t>
+  </si>
+  <si>
+    <t>Crus_II_avg</t>
+  </si>
+  <si>
+    <t>VIIb_avg</t>
+  </si>
+  <si>
+    <t>VIIIa_avg</t>
+  </si>
+  <si>
+    <t>VIIIb_avg</t>
+  </si>
+  <si>
+    <t>IX_avg</t>
+  </si>
+  <si>
+    <t>X_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VI_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIa_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIb_avg</t>
+  </si>
+  <si>
+    <t>Vermis_IX_avg</t>
+  </si>
+  <si>
+    <t>IV_avg</t>
+  </si>
+  <si>
+    <t>V_avg</t>
+  </si>
+  <si>
+    <t>VI_avg</t>
+  </si>
+  <si>
+    <t>Crus_I_avg</t>
+  </si>
+  <si>
+    <t>Crus_II_avg</t>
+  </si>
+  <si>
+    <t>VIIb_avg</t>
+  </si>
+  <si>
+    <t>VIIIa_avg</t>
+  </si>
+  <si>
+    <t>VIIIb_avg</t>
+  </si>
+  <si>
+    <t>IX_avg</t>
+  </si>
+  <si>
+    <t>X_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VI_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIa_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIb_avg</t>
+  </si>
+  <si>
+    <t>Vermis_IX_avg</t>
+  </si>
+  <si>
+    <t>IV_avg</t>
+  </si>
+  <si>
+    <t>V_avg</t>
+  </si>
+  <si>
+    <t>VI_avg</t>
+  </si>
+  <si>
+    <t>Crus_I_avg</t>
+  </si>
+  <si>
+    <t>Crus_II_avg</t>
+  </si>
+  <si>
+    <t>VIIb_avg</t>
+  </si>
+  <si>
+    <t>VIIIa_avg</t>
+  </si>
+  <si>
+    <t>VIIIb_avg</t>
+  </si>
+  <si>
+    <t>IX_avg</t>
+  </si>
+  <si>
+    <t>X_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VI_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIa_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIb_avg</t>
+  </si>
+  <si>
+    <t>Vermis_IX_avg</t>
+  </si>
+  <si>
+    <t>IV_avg</t>
+  </si>
+  <si>
+    <t>V_avg</t>
+  </si>
+  <si>
+    <t>VI_avg</t>
+  </si>
+  <si>
+    <t>Crus_I_avg</t>
+  </si>
+  <si>
+    <t>Crus_II_avg</t>
+  </si>
+  <si>
+    <t>VIIb_avg</t>
+  </si>
+  <si>
+    <t>VIIIa_avg</t>
+  </si>
+  <si>
+    <t>VIIIb_avg</t>
+  </si>
+  <si>
+    <t>IX_avg</t>
+  </si>
+  <si>
+    <t>X_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VI_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIa_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIb_avg</t>
+  </si>
+  <si>
+    <t>Vermis_IX_avg</t>
+  </si>
+  <si>
+    <t>IV_avg</t>
+  </si>
+  <si>
+    <t>V_avg</t>
+  </si>
+  <si>
+    <t>VI_avg</t>
+  </si>
+  <si>
+    <t>Crus_I_avg</t>
+  </si>
+  <si>
+    <t>Crus_II_avg</t>
+  </si>
+  <si>
+    <t>VIIb_avg</t>
+  </si>
+  <si>
+    <t>VIIIa_avg</t>
+  </si>
+  <si>
+    <t>VIIIb_avg</t>
+  </si>
+  <si>
+    <t>IX_avg</t>
+  </si>
+  <si>
+    <t>X_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VI_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIa_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIb_avg</t>
+  </si>
+  <si>
+    <t>Vermis_IX_avg</t>
+  </si>
+  <si>
+    <t>IV_avg</t>
+  </si>
+  <si>
+    <t>V_avg</t>
+  </si>
+  <si>
+    <t>VI_avg</t>
+  </si>
+  <si>
+    <t>Crus_I_avg</t>
+  </si>
+  <si>
+    <t>Crus_II_avg</t>
+  </si>
+  <si>
+    <t>VIIb_avg</t>
+  </si>
+  <si>
+    <t>VIIIa_avg</t>
+  </si>
+  <si>
+    <t>VIIIb_avg</t>
+  </si>
+  <si>
+    <t>IX_avg</t>
+  </si>
+  <si>
+    <t>X_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VI_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIa_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIb_avg</t>
+  </si>
+  <si>
+    <t>Vermis_IX_avg</t>
+  </si>
+  <si>
+    <t>IV_avg</t>
+  </si>
+  <si>
+    <t>V_avg</t>
+  </si>
+  <si>
+    <t>VI_avg</t>
+  </si>
+  <si>
+    <t>Crus_I_avg</t>
+  </si>
+  <si>
+    <t>Crus_II_avg</t>
+  </si>
+  <si>
+    <t>VIIb_avg</t>
+  </si>
+  <si>
+    <t>VIIIa_avg</t>
+  </si>
+  <si>
+    <t>VIIIb_avg</t>
+  </si>
+  <si>
+    <t>IX_avg</t>
+  </si>
+  <si>
+    <t>X_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VI_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIa_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIb_avg</t>
+  </si>
+  <si>
+    <t>Vermis_IX_avg</t>
+  </si>
+  <si>
+    <t>IV_avg</t>
+  </si>
+  <si>
+    <t>V_avg</t>
+  </si>
+  <si>
+    <t>VI_avg</t>
+  </si>
+  <si>
+    <t>Crus_I_avg</t>
+  </si>
+  <si>
+    <t>Crus_II_avg</t>
+  </si>
+  <si>
+    <t>VIIb_avg</t>
+  </si>
+  <si>
+    <t>VIIIa_avg</t>
+  </si>
+  <si>
+    <t>VIIIb_avg</t>
+  </si>
+  <si>
+    <t>IX_avg</t>
+  </si>
+  <si>
+    <t>X_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VI_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIa_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIb_avg</t>
+  </si>
+  <si>
+    <t>Vermis_IX_avg</t>
+  </si>
+  <si>
+    <t>IV_avg</t>
+  </si>
+  <si>
+    <t>V_avg</t>
+  </si>
+  <si>
+    <t>VI_avg</t>
+  </si>
+  <si>
+    <t>Crus_I_avg</t>
+  </si>
+  <si>
+    <t>Crus_II_avg</t>
+  </si>
+  <si>
+    <t>VIIb_avg</t>
+  </si>
+  <si>
+    <t>VIIIa_avg</t>
+  </si>
+  <si>
+    <t>VIIIb_avg</t>
+  </si>
+  <si>
+    <t>IX_avg</t>
+  </si>
+  <si>
+    <t>X_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VI_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIa_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIb_avg</t>
+  </si>
+  <si>
+    <t>Vermis_IX_avg</t>
+  </si>
+  <si>
+    <t>IV_avg</t>
+  </si>
+  <si>
+    <t>V_avg</t>
+  </si>
+  <si>
+    <t>VI_avg</t>
+  </si>
+  <si>
+    <t>Crus_I_avg</t>
+  </si>
+  <si>
+    <t>Crus_II_avg</t>
+  </si>
+  <si>
+    <t>VIIb_avg</t>
+  </si>
+  <si>
+    <t>VIIIa_avg</t>
+  </si>
+  <si>
+    <t>VIIIb_avg</t>
+  </si>
+  <si>
+    <t>IX_avg</t>
+  </si>
+  <si>
+    <t>X_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VI_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIa_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIb_avg</t>
+  </si>
+  <si>
+    <t>Vermis_IX_avg</t>
+  </si>
+  <si>
+    <t>IV_avg</t>
+  </si>
+  <si>
+    <t>V_avg</t>
+  </si>
+  <si>
+    <t>VI_avg</t>
+  </si>
+  <si>
+    <t>Crus_I_avg</t>
+  </si>
+  <si>
+    <t>Crus_II_avg</t>
+  </si>
+  <si>
+    <t>VIIb_avg</t>
+  </si>
+  <si>
+    <t>VIIIa_avg</t>
+  </si>
+  <si>
+    <t>VIIIb_avg</t>
+  </si>
+  <si>
+    <t>IX_avg</t>
+  </si>
+  <si>
+    <t>X_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VI_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIa_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIb_avg</t>
+  </si>
+  <si>
+    <t>Vermis_IX_avg</t>
+  </si>
+  <si>
+    <t>IV_avg</t>
+  </si>
+  <si>
+    <t>V_avg</t>
+  </si>
+  <si>
+    <t>VI_avg</t>
+  </si>
+  <si>
+    <t>Crus_I_avg</t>
+  </si>
+  <si>
+    <t>Crus_II_avg</t>
+  </si>
+  <si>
+    <t>VIIb_avg</t>
+  </si>
+  <si>
+    <t>VIIIa_avg</t>
+  </si>
+  <si>
+    <t>VIIIb_avg</t>
+  </si>
+  <si>
+    <t>IX_avg</t>
+  </si>
+  <si>
+    <t>X_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VI_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIa_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIb_avg</t>
+  </si>
+  <si>
+    <t>Vermis_IX_avg</t>
+  </si>
+  <si>
+    <t>IV_avg</t>
+  </si>
+  <si>
+    <t>V_avg</t>
+  </si>
+  <si>
+    <t>VI_avg</t>
+  </si>
+  <si>
+    <t>Crus_I_avg</t>
+  </si>
+  <si>
+    <t>Crus_II_avg</t>
+  </si>
+  <si>
+    <t>VIIb_avg</t>
+  </si>
+  <si>
+    <t>VIIIa_avg</t>
+  </si>
+  <si>
+    <t>VIIIb_avg</t>
+  </si>
+  <si>
+    <t>IX_avg</t>
+  </si>
+  <si>
+    <t>X_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VI_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIa_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIb_avg</t>
+  </si>
+  <si>
+    <t>Vermis_IX_avg</t>
+  </si>
+  <si>
+    <t>IV_avg</t>
+  </si>
+  <si>
+    <t>V_avg</t>
+  </si>
+  <si>
+    <t>VI_avg</t>
+  </si>
+  <si>
+    <t>Crus_I_avg</t>
+  </si>
+  <si>
+    <t>Crus_II_avg</t>
+  </si>
+  <si>
+    <t>VIIb_avg</t>
+  </si>
+  <si>
+    <t>VIIIa_avg</t>
+  </si>
+  <si>
+    <t>VIIIb_avg</t>
+  </si>
+  <si>
+    <t>IX_avg</t>
+  </si>
+  <si>
+    <t>X_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VI_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIa_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIb_avg</t>
+  </si>
+  <si>
+    <t>Vermis_IX_avg</t>
+  </si>
+  <si>
+    <t>IV_avg</t>
+  </si>
+  <si>
+    <t>V_avg</t>
+  </si>
+  <si>
+    <t>VI_avg</t>
+  </si>
+  <si>
+    <t>Crus_I_avg</t>
+  </si>
+  <si>
+    <t>Crus_II_avg</t>
+  </si>
+  <si>
+    <t>VIIb_avg</t>
+  </si>
+  <si>
+    <t>VIIIa_avg</t>
+  </si>
+  <si>
+    <t>VIIIb_avg</t>
+  </si>
+  <si>
+    <t>IX_avg</t>
+  </si>
+  <si>
+    <t>X_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VI_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIa_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIb_avg</t>
+  </si>
+  <si>
+    <t>Vermis_IX_avg</t>
+  </si>
+  <si>
+    <t>IV_avg</t>
+  </si>
+  <si>
+    <t>V_avg</t>
+  </si>
+  <si>
+    <t>VI_avg</t>
+  </si>
+  <si>
+    <t>Crus_I_avg</t>
+  </si>
+  <si>
+    <t>Crus_II_avg</t>
+  </si>
+  <si>
+    <t>VIIb_avg</t>
+  </si>
+  <si>
+    <t>VIIIa_avg</t>
+  </si>
+  <si>
+    <t>VIIIb_avg</t>
+  </si>
+  <si>
+    <t>IX_avg</t>
+  </si>
+  <si>
+    <t>X_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VI_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIa_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIb_avg</t>
+  </si>
+  <si>
+    <t>Vermis_IX_avg</t>
+  </si>
+  <si>
+    <t>IV_avg</t>
+  </si>
+  <si>
+    <t>V_avg</t>
+  </si>
+  <si>
+    <t>VI_avg</t>
+  </si>
+  <si>
+    <t>Crus_I_avg</t>
+  </si>
+  <si>
+    <t>Crus_II_avg</t>
+  </si>
+  <si>
+    <t>VIIb_avg</t>
+  </si>
+  <si>
+    <t>VIIIa_avg</t>
+  </si>
+  <si>
+    <t>VIIIb_avg</t>
+  </si>
+  <si>
+    <t>IX_avg</t>
+  </si>
+  <si>
+    <t>X_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VI_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIa_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIb_avg</t>
+  </si>
+  <si>
+    <t>Vermis_IX_avg</t>
+  </si>
+  <si>
+    <t>IV_avg</t>
+  </si>
+  <si>
+    <t>V_avg</t>
+  </si>
+  <si>
+    <t>VI_avg</t>
+  </si>
+  <si>
+    <t>Crus_I_avg</t>
+  </si>
+  <si>
+    <t>Crus_II_avg</t>
+  </si>
+  <si>
+    <t>VIIb_avg</t>
+  </si>
+  <si>
+    <t>VIIIa_avg</t>
+  </si>
+  <si>
+    <t>VIIIb_avg</t>
+  </si>
+  <si>
+    <t>IX_avg</t>
+  </si>
+  <si>
+    <t>X_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VI_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIa_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIb_avg</t>
+  </si>
+  <si>
+    <t>Vermis_IX_avg</t>
+  </si>
+  <si>
+    <t>IV_avg</t>
+  </si>
+  <si>
+    <t>V_avg</t>
+  </si>
+  <si>
+    <t>VI_avg</t>
+  </si>
+  <si>
+    <t>Crus_I_avg</t>
+  </si>
+  <si>
+    <t>Crus_II_avg</t>
+  </si>
+  <si>
+    <t>VIIb_avg</t>
+  </si>
+  <si>
+    <t>VIIIa_avg</t>
+  </si>
+  <si>
+    <t>VIIIb_avg</t>
+  </si>
+  <si>
+    <t>IX_avg</t>
+  </si>
+  <si>
+    <t>X_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VI_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIa_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIb_avg</t>
+  </si>
+  <si>
+    <t>Vermis_IX_avg</t>
+  </si>
+  <si>
+    <t>IV_avg</t>
+  </si>
+  <si>
+    <t>V_avg</t>
+  </si>
+  <si>
+    <t>VI_avg</t>
+  </si>
+  <si>
+    <t>Crus_I_avg</t>
+  </si>
+  <si>
+    <t>Crus_II_avg</t>
+  </si>
+  <si>
+    <t>VIIb_avg</t>
+  </si>
+  <si>
+    <t>VIIIa_avg</t>
+  </si>
+  <si>
+    <t>VIIIb_avg</t>
+  </si>
+  <si>
+    <t>IX_avg</t>
+  </si>
+  <si>
+    <t>X_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VI_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIa_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIb_avg</t>
+  </si>
+  <si>
+    <t>Vermis_IX_avg</t>
+  </si>
+  <si>
+    <t>IV_avg</t>
+  </si>
+  <si>
+    <t>V_avg</t>
+  </si>
+  <si>
+    <t>VI_avg</t>
+  </si>
+  <si>
+    <t>Crus_I_avg</t>
+  </si>
+  <si>
+    <t>Crus_II_avg</t>
+  </si>
+  <si>
+    <t>VIIb_avg</t>
+  </si>
+  <si>
+    <t>VIIIa_avg</t>
+  </si>
+  <si>
+    <t>VIIIb_avg</t>
+  </si>
+  <si>
+    <t>IX_avg</t>
+  </si>
+  <si>
+    <t>X_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VI_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIa_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIb_avg</t>
+  </si>
+  <si>
+    <t>Vermis_IX_avg</t>
+  </si>
+  <si>
+    <t>IV_avg</t>
+  </si>
+  <si>
+    <t>V_avg</t>
+  </si>
+  <si>
+    <t>VI_avg</t>
+  </si>
+  <si>
+    <t>Crus_I_avg</t>
+  </si>
+  <si>
+    <t>Crus_II_avg</t>
+  </si>
+  <si>
+    <t>VIIb_avg</t>
+  </si>
+  <si>
+    <t>VIIIa_avg</t>
+  </si>
+  <si>
+    <t>VIIIb_avg</t>
+  </si>
+  <si>
+    <t>IX_avg</t>
+  </si>
+  <si>
+    <t>X_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VI_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIa_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIb_avg</t>
+  </si>
+  <si>
+    <t>Vermis_IX_avg</t>
+  </si>
+  <si>
+    <t>IV_avg</t>
+  </si>
+  <si>
+    <t>V_avg</t>
+  </si>
+  <si>
+    <t>VI_avg</t>
+  </si>
+  <si>
+    <t>Crus_I_avg</t>
+  </si>
+  <si>
+    <t>Crus_II_avg</t>
+  </si>
+  <si>
+    <t>VIIb_avg</t>
+  </si>
+  <si>
+    <t>VIIIa_avg</t>
+  </si>
+  <si>
+    <t>VIIIb_avg</t>
+  </si>
+  <si>
+    <t>IX_avg</t>
+  </si>
+  <si>
+    <t>X_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VI_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIa_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIb_avg</t>
+  </si>
+  <si>
+    <t>Vermis_IX_avg</t>
+  </si>
+  <si>
+    <t>IV_avg</t>
+  </si>
+  <si>
+    <t>V_avg</t>
+  </si>
+  <si>
+    <t>VI_avg</t>
+  </si>
+  <si>
+    <t>Crus_I_avg</t>
+  </si>
+  <si>
+    <t>Crus_II_avg</t>
+  </si>
+  <si>
+    <t>VIIb_avg</t>
+  </si>
+  <si>
+    <t>VIIIa_avg</t>
+  </si>
+  <si>
+    <t>VIIIb_avg</t>
+  </si>
+  <si>
+    <t>IX_avg</t>
+  </si>
+  <si>
+    <t>X_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VI_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIa_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIb_avg</t>
+  </si>
+  <si>
+    <t>Vermis_IX_avg</t>
+  </si>
+  <si>
+    <t>IV_avg</t>
+  </si>
+  <si>
+    <t>V_avg</t>
+  </si>
+  <si>
+    <t>VI_avg</t>
+  </si>
+  <si>
+    <t>Crus_I_avg</t>
+  </si>
+  <si>
+    <t>Crus_II_avg</t>
+  </si>
+  <si>
+    <t>VIIb_avg</t>
+  </si>
+  <si>
+    <t>VIIIa_avg</t>
+  </si>
+  <si>
+    <t>VIIIb_avg</t>
+  </si>
+  <si>
+    <t>IX_avg</t>
+  </si>
+  <si>
+    <t>X_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VI_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIa_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIb_avg</t>
+  </si>
+  <si>
+    <t>Vermis_IX_avg</t>
+  </si>
+  <si>
+    <t>IV_avg</t>
+  </si>
+  <si>
+    <t>V_avg</t>
+  </si>
+  <si>
+    <t>VI_avg</t>
+  </si>
+  <si>
+    <t>Crus_I_avg</t>
+  </si>
+  <si>
+    <t>Crus_II_avg</t>
+  </si>
+  <si>
+    <t>VIIb_avg</t>
+  </si>
+  <si>
+    <t>VIIIa_avg</t>
+  </si>
+  <si>
+    <t>VIIIb_avg</t>
+  </si>
+  <si>
+    <t>IX_avg</t>
+  </si>
+  <si>
+    <t>X_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VI_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIa_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIb_avg</t>
+  </si>
+  <si>
+    <t>Vermis_IX_avg</t>
+  </si>
+  <si>
+    <t>IV_avg</t>
+  </si>
+  <si>
+    <t>V_avg</t>
+  </si>
+  <si>
+    <t>VI_avg</t>
+  </si>
+  <si>
+    <t>Crus_I_avg</t>
+  </si>
+  <si>
+    <t>Crus_II_avg</t>
+  </si>
+  <si>
+    <t>VIIb_avg</t>
+  </si>
+  <si>
+    <t>VIIIa_avg</t>
+  </si>
+  <si>
+    <t>VIIIb_avg</t>
+  </si>
+  <si>
+    <t>IX_avg</t>
+  </si>
+  <si>
+    <t>X_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VI_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIa_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIb_avg</t>
+  </si>
+  <si>
+    <t>Vermis_IX_avg</t>
+  </si>
+  <si>
+    <t>IV_avg</t>
+  </si>
+  <si>
+    <t>V_avg</t>
+  </si>
+  <si>
+    <t>VI_avg</t>
+  </si>
+  <si>
+    <t>Crus_I_avg</t>
+  </si>
+  <si>
+    <t>Crus_II_avg</t>
+  </si>
+  <si>
+    <t>VIIb_avg</t>
+  </si>
+  <si>
+    <t>VIIIa_avg</t>
+  </si>
+  <si>
+    <t>VIIIb_avg</t>
+  </si>
+  <si>
+    <t>IX_avg</t>
+  </si>
+  <si>
+    <t>X_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VI_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIa_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIb_avg</t>
+  </si>
+  <si>
+    <t>Vermis_IX_avg</t>
+  </si>
+  <si>
+    <t>IV_avg</t>
+  </si>
+  <si>
+    <t>V_avg</t>
+  </si>
+  <si>
+    <t>VI_avg</t>
+  </si>
+  <si>
+    <t>Crus_I_avg</t>
+  </si>
+  <si>
+    <t>Crus_II_avg</t>
+  </si>
+  <si>
+    <t>VIIb_avg</t>
+  </si>
+  <si>
+    <t>VIIIa_avg</t>
+  </si>
+  <si>
+    <t>VIIIb_avg</t>
+  </si>
+  <si>
+    <t>IX_avg</t>
+  </si>
+  <si>
+    <t>X_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VI_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIa_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIb_avg</t>
+  </si>
+  <si>
+    <t>Vermis_IX_avg</t>
+  </si>
+  <si>
+    <t>IV_avg</t>
+  </si>
+  <si>
+    <t>V_avg</t>
+  </si>
+  <si>
+    <t>VI_avg</t>
+  </si>
+  <si>
+    <t>Crus_I_avg</t>
+  </si>
+  <si>
+    <t>Crus_II_avg</t>
+  </si>
+  <si>
+    <t>VIIb_avg</t>
+  </si>
+  <si>
+    <t>VIIIa_avg</t>
+  </si>
+  <si>
+    <t>VIIIb_avg</t>
+  </si>
+  <si>
+    <t>IX_avg</t>
+  </si>
+  <si>
+    <t>X_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VI_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIa_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIb_avg</t>
+  </si>
+  <si>
+    <t>Vermis_IX_avg</t>
+  </si>
+  <si>
+    <t>IV_avg</t>
+  </si>
+  <si>
+    <t>V_avg</t>
+  </si>
+  <si>
+    <t>VI_avg</t>
+  </si>
+  <si>
+    <t>Crus_I_avg</t>
+  </si>
+  <si>
+    <t>Crus_II_avg</t>
+  </si>
+  <si>
+    <t>VIIb_avg</t>
+  </si>
+  <si>
+    <t>VIIIa_avg</t>
+  </si>
+  <si>
+    <t>VIIIb_avg</t>
+  </si>
+  <si>
+    <t>IX_avg</t>
+  </si>
+  <si>
+    <t>X_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VI_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIa_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIb_avg</t>
+  </si>
+  <si>
+    <t>Vermis_IX_avg</t>
+  </si>
+  <si>
+    <t>IV_avg</t>
+  </si>
+  <si>
+    <t>V_avg</t>
+  </si>
+  <si>
+    <t>VI_avg</t>
+  </si>
+  <si>
+    <t>Crus_I_avg</t>
+  </si>
+  <si>
+    <t>Crus_II_avg</t>
+  </si>
+  <si>
+    <t>VIIb_avg</t>
+  </si>
+  <si>
+    <t>VIIIa_avg</t>
+  </si>
+  <si>
+    <t>VIIIb_avg</t>
+  </si>
+  <si>
+    <t>IX_avg</t>
+  </si>
+  <si>
+    <t>X_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VI_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIa_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIb_avg</t>
+  </si>
+  <si>
+    <t>Vermis_IX_avg</t>
+  </si>
   <si>
     <t>IV_avg</t>
   </si>
@@ -751,46 +2137,46 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>210</v>
+        <v>672</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>211</v>
+        <v>673</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>212</v>
+        <v>674</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>213</v>
+        <v>675</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>214</v>
+        <v>676</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>215</v>
+        <v>677</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>216</v>
+        <v>678</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>217</v>
+        <v>679</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>218</v>
+        <v>680</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>219</v>
+        <v>681</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>220</v>
+        <v>682</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>221</v>
+        <v>683</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>222</v>
+        <v>684</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>223</v>
+        <v>685</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
prep palm for 2>1 with GSR
</commit_message>
<xml_diff>
--- a/code/h1_data_left.xlsx
+++ b/code/h1_data_left.xlsx
@@ -13,7 +13,133 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="882">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="924">
+  <si>
+    <t>IV_avg</t>
+  </si>
+  <si>
+    <t>V_avg</t>
+  </si>
+  <si>
+    <t>VI_avg</t>
+  </si>
+  <si>
+    <t>Crus_I_avg</t>
+  </si>
+  <si>
+    <t>Crus_II_avg</t>
+  </si>
+  <si>
+    <t>VIIb_avg</t>
+  </si>
+  <si>
+    <t>VIIIa_avg</t>
+  </si>
+  <si>
+    <t>VIIIb_avg</t>
+  </si>
+  <si>
+    <t>IX_avg</t>
+  </si>
+  <si>
+    <t>X_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VI_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIa_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIb_avg</t>
+  </si>
+  <si>
+    <t>Vermis_IX_avg</t>
+  </si>
+  <si>
+    <t>IV_avg</t>
+  </si>
+  <si>
+    <t>V_avg</t>
+  </si>
+  <si>
+    <t>VI_avg</t>
+  </si>
+  <si>
+    <t>Crus_I_avg</t>
+  </si>
+  <si>
+    <t>Crus_II_avg</t>
+  </si>
+  <si>
+    <t>VIIb_avg</t>
+  </si>
+  <si>
+    <t>VIIIa_avg</t>
+  </si>
+  <si>
+    <t>VIIIb_avg</t>
+  </si>
+  <si>
+    <t>IX_avg</t>
+  </si>
+  <si>
+    <t>X_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VI_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIa_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIb_avg</t>
+  </si>
+  <si>
+    <t>Vermis_IX_avg</t>
+  </si>
+  <si>
+    <t>IV_avg</t>
+  </si>
+  <si>
+    <t>V_avg</t>
+  </si>
+  <si>
+    <t>VI_avg</t>
+  </si>
+  <si>
+    <t>Crus_I_avg</t>
+  </si>
+  <si>
+    <t>Crus_II_avg</t>
+  </si>
+  <si>
+    <t>VIIb_avg</t>
+  </si>
+  <si>
+    <t>VIIIa_avg</t>
+  </si>
+  <si>
+    <t>VIIIb_avg</t>
+  </si>
+  <si>
+    <t>IX_avg</t>
+  </si>
+  <si>
+    <t>X_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VI_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIa_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIb_avg</t>
+  </si>
+  <si>
+    <t>Vermis_IX_avg</t>
+  </si>
   <si>
     <t>IV_avg</t>
   </si>
@@ -2725,46 +2851,46 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>868</v>
+        <v>910</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>869</v>
+        <v>911</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>870</v>
+        <v>912</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>871</v>
+        <v>913</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>872</v>
+        <v>914</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>873</v>
+        <v>915</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>874</v>
+        <v>916</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>875</v>
+        <v>917</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>876</v>
+        <v>918</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>877</v>
+        <v>919</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>878</v>
+        <v>920</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>879</v>
+        <v>921</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>880</v>
+        <v>922</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>881</v>
+        <v>923</v>
       </c>
     </row>
     <row r="2">

</xml_diff>